<commit_message>
Made changes on features files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLoader/GenericUploader/NoTool/Excel/Action.xlsx
+++ b/src/test/resources/testdata/DataLoader/GenericUploader/NoTool/Excel/Action.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="597">
   <si>
     <t>Title</t>
   </si>
@@ -2350,6 +2350,12 @@
   </si>
   <si>
     <t>30053</t>
+  </si>
+  <si>
+    <t>18858</t>
+  </si>
+  <si>
+    <t>18360</t>
   </si>
 </sst>
 </file>
@@ -7241,7 +7247,7 @@
     </row>
     <row r="2" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="11" t="s">

</xml_diff>

<commit_message>
Server IB Create Log in Extent Report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLoader/GenericUploader/NoTool/Excel/Action.xlsx
+++ b/src/test/resources/testdata/DataLoader/GenericUploader/NoTool/Excel/Action.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="607">
   <si>
     <t>Title</t>
   </si>
@@ -2383,6 +2383,9 @@
   </si>
   <si>
     <t>35037</t>
+  </si>
+  <si>
+    <t>91765</t>
   </si>
 </sst>
 </file>
@@ -7274,7 +7277,7 @@
     </row>
     <row r="2" spans="1:91" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="11" t="s">

</xml_diff>